<commit_message>
Edit Cost Calculation and combined data
</commit_message>
<xml_diff>
--- a/Data/Cost Calculation.xlsx
+++ b/Data/Cost Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\soiSMA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D543A57-E89F-416D-9ECC-B67E30723A1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B70FA6-A765-48A7-9B94-0FF3B32D16ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{3655CA4D-2F4C-4629-AA28-842FC012CC9E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="92">
   <si>
     <t>Item Code (on menu)</t>
   </si>
@@ -257,6 +257,60 @@
   </si>
   <si>
     <t xml:space="preserve">Creamy Tom Yum </t>
+  </si>
+  <si>
+    <t>Tom Yum Gong</t>
+  </si>
+  <si>
+    <t>QUANTITY SOLD</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan </t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>COST</t>
+  </si>
+  <si>
+    <t>TOTAL COST</t>
+  </si>
+  <si>
+    <t>SPICY</t>
+  </si>
+  <si>
+    <t>NON-SPICY</t>
   </si>
 </sst>
 </file>
@@ -266,7 +320,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +347,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -584,34 +644,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -627,15 +663,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -671,10 +698,50 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -992,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A003CE-6C0D-43F3-AEDF-E280FF96892A}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView zoomScale="84" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView topLeftCell="A32" zoomScale="84" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1010,1615 +1077,1622 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="21">
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="10">
         <v>200</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="9">
         <f>(E2/VLOOKUP(C2,$J$2:$L$27,2,FALSE))*VLOOKUP(C2,$J$2:$L$27,3,FALSE)</f>
         <v>3.6</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="22">
         <f>SUM(F2:F8)</f>
         <v>5.1350000000000007</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="22">
+      <c r="K2" s="11">
         <v>1000</v>
       </c>
-      <c r="L2" s="26">
+      <c r="L2" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="8"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="11">
         <v>0.5</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="9">
         <f t="shared" ref="F3:F66" si="0">(E3/VLOOKUP(C3,$J$2:$L$27,2,FALSE))*VLOOKUP(C3,$J$2:$L$27,3,FALSE)</f>
         <v>0.1</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="J3" s="24" t="s">
+      <c r="G3" s="23"/>
+      <c r="J3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="22">
+      <c r="K3" s="11">
         <v>1</v>
       </c>
-      <c r="L3" s="26">
+      <c r="L3" s="15">
         <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="8"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="22">
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="11">
         <v>15</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="9">
         <f t="shared" si="0"/>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="J4" s="24" t="s">
+      <c r="G4" s="23"/>
+      <c r="J4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="22">
+      <c r="K4" s="11">
         <v>100</v>
       </c>
-      <c r="L4" s="26">
+      <c r="L4" s="15">
         <v>1.8</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="8"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="22">
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="11">
         <v>10</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="9">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="J5" s="24" t="s">
+      <c r="G5" s="23"/>
+      <c r="J5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="22">
+      <c r="K5" s="11">
         <v>100</v>
       </c>
-      <c r="L5" s="26">
+      <c r="L5" s="15">
         <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="8"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2" t="s">
+      <c r="A6" s="26"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="22">
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="11">
         <v>200</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="9">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="J6" s="24" t="s">
+      <c r="G6" s="23"/>
+      <c r="J6" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="K6" s="22">
+      <c r="K6" s="11">
         <v>1000</v>
       </c>
-      <c r="L6" s="26">
+      <c r="L6" s="15">
         <v>3.5</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="8"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="22">
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="11">
         <v>20</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="9">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="J7" s="24" t="s">
+      <c r="G7" s="23"/>
+      <c r="J7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="22">
+      <c r="K7" s="11">
         <v>1000</v>
       </c>
-      <c r="L7" s="26">
+      <c r="L7" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11" t="s">
+      <c r="A8" s="27"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="23">
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="12">
         <v>80</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="19">
         <f t="shared" si="0"/>
         <v>0.32000000000000006</v>
       </c>
-      <c r="G8" s="19"/>
-      <c r="J8" s="24" t="s">
+      <c r="G8" s="24"/>
+      <c r="J8" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="22">
+      <c r="K8" s="11">
         <v>1000</v>
       </c>
-      <c r="L8" s="26">
+      <c r="L8" s="15">
         <v>3.5</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="21">
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="10">
         <v>50</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="9">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="22">
         <f>SUM(F9:F16)</f>
         <v>1.0385000000000002</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="J9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="22">
+      <c r="K9" s="11">
         <v>100</v>
       </c>
-      <c r="L9" s="26">
+      <c r="L9" s="15">
         <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="8"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2" t="s">
+      <c r="A10" s="26"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="11">
         <v>0.5</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="9">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="J10" s="24" t="s">
+      <c r="G10" s="23"/>
+      <c r="J10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="22">
+      <c r="K10" s="11">
         <v>100</v>
       </c>
-      <c r="L10" s="26">
+      <c r="L10" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="8"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2" t="s">
+      <c r="A11" s="26"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="22">
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="11">
         <v>15</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="9">
         <f t="shared" si="0"/>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="J11" s="24" t="s">
+      <c r="G11" s="23"/>
+      <c r="J11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="11">
         <v>1000</v>
       </c>
-      <c r="L11" s="26">
+      <c r="L11" s="15">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="8"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="2" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="22">
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="11">
         <v>30</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="9">
         <f t="shared" si="0"/>
         <v>0.105</v>
       </c>
-      <c r="G12" s="18"/>
-      <c r="J12" s="24" t="s">
+      <c r="G12" s="23"/>
+      <c r="J12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="11">
         <v>1000</v>
       </c>
-      <c r="L12" s="26">
+      <c r="L12" s="15">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="8"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="22">
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="11">
         <v>20</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="9">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-      <c r="G13" s="18"/>
-      <c r="J13" s="24" t="s">
+      <c r="G13" s="23"/>
+      <c r="J13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="11">
         <v>100</v>
       </c>
-      <c r="L13" s="26">
+      <c r="L13" s="15">
         <v>1.5</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="8"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2" t="s">
+      <c r="A14" s="26"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="22">
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="11">
         <v>30</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="9">
         <f t="shared" si="0"/>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="G14" s="18"/>
-      <c r="J14" s="24" t="s">
+      <c r="G14" s="23"/>
+      <c r="J14" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="22">
+      <c r="K14" s="11">
         <v>1000</v>
       </c>
-      <c r="L14" s="26">
+      <c r="L14" s="15">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="8"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="2" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="22">
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="11">
         <v>80</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="9">
         <f t="shared" si="0"/>
         <v>0.32000000000000006</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="J15" s="24" t="s">
+      <c r="G15" s="23"/>
+      <c r="J15" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="22">
+      <c r="K15" s="11">
         <v>1000</v>
       </c>
-      <c r="L15" s="26">
+      <c r="L15" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11" t="s">
+      <c r="A16" s="27"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="23">
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="12">
         <v>15</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="19">
         <f t="shared" si="0"/>
         <v>5.2499999999999998E-2</v>
       </c>
-      <c r="G16" s="19"/>
-      <c r="J16" s="24" t="s">
+      <c r="G16" s="24"/>
+      <c r="J16" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="K16" s="22">
+      <c r="K16" s="11">
         <v>1000</v>
       </c>
-      <c r="L16" s="26">
+      <c r="L16" s="15">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="21">
+      <c r="D17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="10">
         <v>150</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="9">
         <f t="shared" si="0"/>
         <v>0.89999999999999991</v>
       </c>
-      <c r="G17" s="17">
+      <c r="G17" s="22">
         <f>SUM(F17:F22)</f>
         <v>2.7320000000000002</v>
       </c>
-      <c r="J17" s="24" t="s">
+      <c r="J17" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="K17" s="22">
+      <c r="K17" s="11">
         <v>1000</v>
       </c>
-      <c r="L17" s="26">
+      <c r="L17" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="8"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="2" t="s">
+      <c r="A18" s="26"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="22">
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="11">
         <v>40</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="9">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="J18" s="24" t="s">
+      <c r="G18" s="23"/>
+      <c r="J18" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="K18" s="22">
+      <c r="K18" s="11">
         <v>1000</v>
       </c>
-      <c r="L18" s="26">
+      <c r="L18" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="8"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="2" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="22">
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="11">
         <v>20</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="9">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="J19" s="24" t="s">
+      <c r="G19" s="23"/>
+      <c r="J19" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="K19" s="22">
+      <c r="K19" s="11">
         <v>1000</v>
       </c>
-      <c r="L19" s="26">
+      <c r="L19" s="15">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="8"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="2" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="22">
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="11">
         <v>30</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="9">
         <f t="shared" si="0"/>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="J20" s="24" t="s">
+      <c r="G20" s="23"/>
+      <c r="J20" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="K20" s="22">
+      <c r="K20" s="11">
         <v>1000</v>
       </c>
-      <c r="L20" s="26">
+      <c r="L20" s="15">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="8"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="2" t="s">
+      <c r="A21" s="26"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="22">
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="11">
         <v>200</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F21" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="J21" s="2" t="s">
+      <c r="G21" s="23"/>
+      <c r="J21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K21" s="28">
+      <c r="K21" s="17">
         <v>1000</v>
       </c>
-      <c r="L21" s="29">
+      <c r="L21" s="18">
         <v>2.4</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="11" t="s">
+      <c r="A22" s="27"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="23">
+      <c r="D22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="12">
         <v>80</v>
       </c>
-      <c r="F22" s="30">
+      <c r="F22" s="19">
         <f t="shared" si="0"/>
         <v>0.32000000000000006</v>
       </c>
-      <c r="G22" s="19"/>
-      <c r="J22" s="27" t="s">
+      <c r="G22" s="24"/>
+      <c r="J22" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="K22" s="28">
+      <c r="K22" s="17">
         <v>1000</v>
       </c>
-      <c r="L22" s="29">
+      <c r="L22" s="18">
         <v>3.2</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="21">
+      <c r="D23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="10">
         <v>200</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G23" s="17">
+      <c r="G23" s="22">
         <f>SUM(F23:F27)</f>
         <v>4.8800000000000008</v>
       </c>
-      <c r="J23" s="27" t="s">
+      <c r="J23" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="K23" s="28">
+      <c r="K23" s="17">
         <v>1000</v>
       </c>
-      <c r="L23" s="29">
+      <c r="L23" s="18">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="8"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="2" t="s">
+      <c r="A24" s="26"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="22">
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="11">
         <v>40</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F24" s="9">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G24" s="18"/>
-      <c r="J24" s="27" t="s">
+      <c r="G24" s="23"/>
+      <c r="J24" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="K24" s="28">
+      <c r="K24" s="17">
         <v>100</v>
       </c>
-      <c r="L24" s="29">
+      <c r="L24" s="18">
         <v>1.8</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="8"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="2" t="s">
+      <c r="A25" s="26"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="22">
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="11">
         <v>200</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="9">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G25" s="18"/>
-      <c r="J25" s="27" t="s">
+      <c r="G25" s="23"/>
+      <c r="J25" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="K25" s="28">
+      <c r="K25" s="17">
         <v>1000</v>
       </c>
-      <c r="L25" s="29">
+      <c r="L25" s="18">
         <v>6.5</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="8"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="2" t="s">
+      <c r="A26" s="26"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="22">
+      <c r="D26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="11">
         <v>20</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="9">
         <f t="shared" si="0"/>
         <v>0.36000000000000004</v>
       </c>
-      <c r="G26" s="18"/>
-      <c r="J26" s="27" t="s">
+      <c r="G26" s="23"/>
+      <c r="J26" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K26" s="28">
+      <c r="K26" s="17">
         <v>100</v>
       </c>
-      <c r="L26" s="29">
+      <c r="L26" s="18">
         <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="9"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="11" t="s">
+      <c r="A27" s="27"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="23">
+      <c r="D27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="12">
         <v>80</v>
       </c>
-      <c r="F27" s="30">
+      <c r="F27" s="19">
         <f t="shared" si="0"/>
         <v>0.32000000000000006</v>
       </c>
-      <c r="G27" s="19"/>
-      <c r="J27" s="27" t="s">
+      <c r="G27" s="24"/>
+      <c r="J27" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="K27" s="28">
+      <c r="K27" s="17">
         <v>1000</v>
       </c>
-      <c r="L27" s="29">
+      <c r="L27" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="21">
+      <c r="D28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="10">
         <v>50</v>
       </c>
-      <c r="F28" s="20">
+      <c r="F28" s="9">
         <f t="shared" si="0"/>
         <v>0.32500000000000001</v>
       </c>
-      <c r="G28" s="17">
+      <c r="G28" s="22">
         <f>SUM(F28:F34)</f>
         <v>1.51</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="8"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="2" t="s">
+      <c r="A29" s="26"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29" s="11">
         <v>0.5</v>
       </c>
-      <c r="F29" s="20">
+      <c r="F29" s="9">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G29" s="18"/>
+      <c r="G29" s="23"/>
     </row>
     <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="8"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="2" t="s">
+      <c r="A30" s="26"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="22">
+      <c r="D30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="11">
         <v>15</v>
       </c>
-      <c r="F30" s="20">
+      <c r="F30" s="9">
         <f t="shared" si="0"/>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G30" s="18"/>
+      <c r="G30" s="23"/>
     </row>
     <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="8"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="2" t="s">
+      <c r="A31" s="26"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="22">
+      <c r="D31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="11">
         <v>10</v>
       </c>
-      <c r="F31" s="20">
+      <c r="F31" s="9">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-      <c r="G31" s="18"/>
+      <c r="G31" s="23"/>
     </row>
     <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="8"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="2" t="s">
+      <c r="A32" s="26"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="22">
+      <c r="D32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="11">
         <v>50</v>
       </c>
-      <c r="F32" s="20">
+      <c r="F32" s="9">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G32" s="18"/>
+      <c r="G32" s="23"/>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="8"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="2" t="s">
+      <c r="A33" s="26"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="22">
+      <c r="D33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="11">
         <v>40</v>
       </c>
-      <c r="F33" s="20">
+      <c r="F33" s="9">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G33" s="18"/>
+      <c r="G33" s="23"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="11" t="s">
+      <c r="A34" s="27"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="23">
+      <c r="D34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="12">
         <v>80</v>
       </c>
-      <c r="F34" s="30">
+      <c r="F34" s="19">
         <f t="shared" si="0"/>
         <v>0.32000000000000006</v>
       </c>
-      <c r="G34" s="19"/>
+      <c r="G34" s="24"/>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="21">
+      <c r="D35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="10">
         <v>80</v>
       </c>
-      <c r="F35" s="20">
+      <c r="F35" s="9">
         <f t="shared" si="0"/>
         <v>1.4400000000000002</v>
       </c>
-      <c r="G35" s="17">
+      <c r="G35" s="22">
         <f>SUM(F35:F40)</f>
         <v>2.7500000000000009</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="8"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="2" t="s">
+      <c r="A36" s="26"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="22">
+      <c r="E36" s="11">
         <v>0.5</v>
       </c>
-      <c r="F36" s="20">
+      <c r="F36" s="9">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G36" s="18"/>
+      <c r="G36" s="23"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="8"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="2" t="s">
+      <c r="A37" s="26"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="22">
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="11">
         <v>10</v>
       </c>
-      <c r="F37" s="20">
+      <c r="F37" s="9">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="G37" s="18"/>
+      <c r="G37" s="23"/>
     </row>
     <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="8"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="2" t="s">
+      <c r="A38" s="26"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="22">
+      <c r="D38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="11">
         <v>10</v>
       </c>
-      <c r="F38" s="20">
+      <c r="F38" s="9">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-      <c r="G38" s="18"/>
+      <c r="G38" s="23"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="8"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="2" t="s">
+      <c r="A39" s="26"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="22">
+      <c r="D39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="11">
         <v>200</v>
       </c>
-      <c r="F39" s="20">
+      <c r="F39" s="9">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G39" s="18"/>
+      <c r="G39" s="23"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="9"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="11" t="s">
+      <c r="A40" s="27"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="23">
+      <c r="D40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="12">
         <v>80</v>
       </c>
-      <c r="F40" s="30">
+      <c r="F40" s="19">
         <f t="shared" si="0"/>
         <v>0.32000000000000006</v>
       </c>
-      <c r="G40" s="19"/>
+      <c r="G40" s="24"/>
     </row>
     <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="21">
+      <c r="D41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="10">
         <v>50</v>
       </c>
-      <c r="F41" s="20">
+      <c r="F41" s="9">
         <f t="shared" si="0"/>
         <v>0.32500000000000001</v>
       </c>
-      <c r="G41" s="17">
+      <c r="G41" s="22">
         <f>SUM(F41:F47)</f>
         <v>2.0600000000000005</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="8"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="2" t="s">
+      <c r="A42" s="26"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="22">
+      <c r="E42" s="11">
         <v>0.5</v>
       </c>
-      <c r="F42" s="20">
+      <c r="F42" s="9">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G42" s="18"/>
+      <c r="G42" s="23"/>
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="8"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="2" t="s">
+      <c r="A43" s="26"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="22">
+      <c r="D43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="11">
         <v>15</v>
       </c>
-      <c r="F43" s="20">
+      <c r="F43" s="9">
         <f t="shared" si="0"/>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G43" s="18"/>
+      <c r="G43" s="23"/>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="8"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="2" t="s">
+      <c r="A44" s="26"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="22">
+      <c r="D44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="11">
         <v>10</v>
       </c>
-      <c r="F44" s="20">
+      <c r="F44" s="9">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-      <c r="G44" s="18"/>
+      <c r="G44" s="23"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="8"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="2" t="s">
+      <c r="A45" s="26"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="22">
+      <c r="D45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="11">
         <v>200</v>
       </c>
-      <c r="F45" s="20">
+      <c r="F45" s="9">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G45" s="18"/>
+      <c r="G45" s="23"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="8"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="2" t="s">
+      <c r="A46" s="26"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="22">
+      <c r="D46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="11">
         <v>40</v>
       </c>
-      <c r="F46" s="20">
+      <c r="F46" s="9">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G46" s="18"/>
+      <c r="G46" s="23"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="9"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="11" t="s">
+      <c r="A47" s="27"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D47" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="23">
+      <c r="D47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="12">
         <v>80</v>
       </c>
-      <c r="F47" s="30">
+      <c r="F47" s="19">
         <f t="shared" si="0"/>
         <v>0.32000000000000006</v>
       </c>
-      <c r="G47" s="19"/>
+      <c r="G47" s="24"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="21">
+      <c r="D48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="10">
         <v>80</v>
       </c>
-      <c r="F48" s="20">
+      <c r="F48" s="9">
         <f t="shared" si="0"/>
         <v>0.64</v>
       </c>
-      <c r="G48" s="17">
+      <c r="G48" s="22">
         <f>SUM(F48:F53)</f>
         <v>1.9720000000000002</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="8"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="2" t="s">
+      <c r="A49" s="26"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="22">
+      <c r="D49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="11">
         <v>80</v>
       </c>
-      <c r="F49" s="20">
+      <c r="F49" s="9">
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
-      <c r="G49" s="18"/>
+      <c r="G49" s="23"/>
     </row>
     <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="8"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="2" t="s">
+      <c r="A50" s="26"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="22">
+      <c r="D50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="11">
         <v>20</v>
       </c>
-      <c r="F50" s="20">
+      <c r="F50" s="9">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G50" s="18"/>
+      <c r="G50" s="23"/>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="8"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="2" t="s">
+      <c r="A51" s="26"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" s="22">
+      <c r="D51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="11">
         <v>30</v>
       </c>
-      <c r="F51" s="20">
+      <c r="F51" s="9">
         <f t="shared" si="0"/>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="G51" s="18"/>
+      <c r="G51" s="23"/>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="8"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="2" t="s">
+      <c r="A52" s="26"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E52" s="22">
+      <c r="D52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="11">
         <v>200</v>
       </c>
-      <c r="F52" s="20">
+      <c r="F52" s="9">
         <f t="shared" si="0"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="G52" s="18"/>
+      <c r="G52" s="23"/>
     </row>
     <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="9"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="11" t="s">
+      <c r="A53" s="27"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="23">
+      <c r="D53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="12">
         <v>80</v>
       </c>
-      <c r="F53" s="30">
+      <c r="F53" s="19">
         <f t="shared" si="0"/>
         <v>0.32000000000000006</v>
       </c>
-      <c r="G53" s="19"/>
+      <c r="G53" s="24"/>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D54" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E54" s="21">
+      <c r="D54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="10">
         <v>80</v>
       </c>
-      <c r="F54" s="20">
+      <c r="F54" s="9">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G54" s="17">
+      <c r="G54" s="22">
         <f>SUM(F54:F58)</f>
         <v>2.052</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="8"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="2" t="s">
+      <c r="A55" s="26"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="22">
+      <c r="E55" s="11">
         <v>0.5</v>
       </c>
-      <c r="F55" s="20">
+      <c r="F55" s="9">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G55" s="18"/>
+      <c r="G55" s="23"/>
     </row>
     <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="8"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="2" t="s">
+      <c r="A56" s="26"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" s="22">
+      <c r="D56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="11">
         <v>30</v>
       </c>
-      <c r="F56" s="20">
+      <c r="F56" s="9">
         <f t="shared" si="0"/>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="G56" s="18"/>
+      <c r="G56" s="23"/>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="8"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="2" t="s">
+      <c r="A57" s="26"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="22">
+      <c r="D57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="11">
         <v>200</v>
       </c>
-      <c r="F57" s="20">
+      <c r="F57" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G57" s="18"/>
+      <c r="G57" s="23"/>
     </row>
     <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="9"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="11" t="s">
+      <c r="A58" s="27"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D58" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E58" s="23">
+      <c r="D58" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="12">
         <v>80</v>
       </c>
-      <c r="F58" s="30">
+      <c r="F58" s="19">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="G58" s="19"/>
+      <c r="G58" s="24"/>
     </row>
     <row r="59" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D59" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E59" s="21">
+      <c r="D59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="10">
         <v>150</v>
       </c>
-      <c r="F59" s="20">
+      <c r="F59" s="9">
         <f t="shared" si="0"/>
         <v>1.05</v>
       </c>
-      <c r="G59" s="17">
+      <c r="G59" s="22">
         <f>SUM(F59:F64)</f>
         <v>2.3945000000000007</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="8"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="2" t="s">
+      <c r="A60" s="26"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E60" s="22">
+      <c r="E60" s="11">
         <v>0.5</v>
       </c>
-      <c r="F60" s="20">
+      <c r="F60" s="9">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G60" s="18"/>
+      <c r="G60" s="23"/>
     </row>
     <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="8"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="2" t="s">
+      <c r="A61" s="26"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E61" s="22">
+      <c r="D61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="11">
         <v>30</v>
       </c>
-      <c r="F61" s="20">
+      <c r="F61" s="9">
         <f t="shared" si="0"/>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="G61" s="18"/>
+      <c r="G61" s="23"/>
     </row>
     <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="8"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="2" t="s">
+      <c r="A62" s="26"/>
+      <c r="B62" s="29"/>
+      <c r="C62" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" s="22">
+      <c r="D62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="11">
         <v>15</v>
       </c>
-      <c r="F62" s="20">
+      <c r="F62" s="9">
         <f t="shared" si="0"/>
         <v>5.2499999999999998E-2</v>
       </c>
-      <c r="G62" s="18"/>
+      <c r="G62" s="23"/>
     </row>
     <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="8"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="2" t="s">
+      <c r="A63" s="26"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E63" s="22">
+      <c r="D63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="11">
         <v>200</v>
       </c>
-      <c r="F63" s="20">
+      <c r="F63" s="9">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G63" s="18"/>
+      <c r="G63" s="23"/>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="9"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="11" t="s">
+      <c r="A64" s="27"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D64" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E64" s="23">
+      <c r="D64" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="12">
         <v>80</v>
       </c>
-      <c r="F64" s="30">
+      <c r="F64" s="19">
         <f t="shared" si="0"/>
         <v>0.32000000000000006</v>
       </c>
-      <c r="G64" s="19"/>
+      <c r="G64" s="24"/>
     </row>
     <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D65" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E65" s="21">
+      <c r="D65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="10">
         <v>80</v>
       </c>
-      <c r="F65" s="20">
+      <c r="F65" s="9">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G65" s="17">
+      <c r="G65" s="22">
         <f>SUM(F65:F71)</f>
         <v>2.7444999999999995</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="8"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="2" t="s">
+      <c r="A66" s="26"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D66" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E66" s="22">
+      <c r="E66" s="11">
         <v>0.5</v>
       </c>
-      <c r="F66" s="20">
+      <c r="F66" s="9">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G66" s="18"/>
+      <c r="G66" s="23"/>
     </row>
     <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="8"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="2" t="s">
+      <c r="A67" s="26"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" s="22">
+      <c r="D67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="11">
         <v>30</v>
       </c>
-      <c r="F67" s="20">
+      <c r="F67" s="9">
         <f t="shared" ref="F67:F71" si="1">(E67/VLOOKUP(C67,$J$2:$L$27,2,FALSE))*VLOOKUP(C67,$J$2:$L$27,3,FALSE)</f>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="G67" s="18"/>
+      <c r="G67" s="23"/>
     </row>
     <row r="68" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="8"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="2" t="s">
+      <c r="A68" s="26"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E68" s="22">
+      <c r="D68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="11">
         <v>15</v>
       </c>
-      <c r="F68" s="20">
+      <c r="F68" s="9">
         <f t="shared" si="1"/>
         <v>5.2499999999999998E-2</v>
       </c>
-      <c r="G68" s="18"/>
+      <c r="G68" s="23"/>
     </row>
     <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="8"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="2" t="s">
+      <c r="A69" s="26"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E69" s="22">
+      <c r="D69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="11">
         <v>200</v>
       </c>
-      <c r="F69" s="20">
+      <c r="F69" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G69" s="18"/>
+      <c r="G69" s="23"/>
     </row>
     <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="8"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="2" t="s">
+      <c r="A70" s="26"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E70" s="22">
+      <c r="D70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="11">
         <v>40</v>
       </c>
-      <c r="F70" s="20">
+      <c r="F70" s="9">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="G70" s="18"/>
+      <c r="G70" s="23"/>
     </row>
     <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="9"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="11" t="s">
+      <c r="A71" s="27"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D71" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E71" s="23">
+      <c r="D71" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="12">
         <v>80</v>
       </c>
-      <c r="F71" s="30">
+      <c r="F71" s="19">
         <f t="shared" si="1"/>
         <v>0.32000000000000006</v>
       </c>
-      <c r="G71" s="19"/>
+      <c r="G71" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="G41:G47"/>
-    <mergeCell ref="G48:G53"/>
-    <mergeCell ref="G54:G58"/>
-    <mergeCell ref="G59:G64"/>
-    <mergeCell ref="G65:G71"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="B9:B16"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="B35:B40"/>
     <mergeCell ref="A59:A64"/>
     <mergeCell ref="B59:B64"/>
     <mergeCell ref="A65:A71"/>
@@ -2635,18 +2709,11 @@
     <mergeCell ref="B48:B53"/>
     <mergeCell ref="A54:A58"/>
     <mergeCell ref="B54:B58"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="B9:B16"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="G41:G47"/>
+    <mergeCell ref="G48:G53"/>
+    <mergeCell ref="G54:G58"/>
+    <mergeCell ref="G59:G64"/>
+    <mergeCell ref="G65:G71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2668,104 +2735,104 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="20">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B4" s="4"/>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="20">
         <v>500</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="20">
         <v>4500</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="3"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="29"/>
+      <c r="C6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="20">
         <v>4000</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="3"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="20">
         <v>10000</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B8" s="3"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="29"/>
+      <c r="C8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="20">
         <v>1000</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="4"/>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="32"/>
+      <c r="C9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="20">
         <v>4500</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="20">
         <v>25000</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B13" s="4"/>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="20">
         <v>22000</v>
       </c>
     </row>
@@ -2783,79 +2850,1753 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B02C95-A6A5-4A71-B182-7BFA47081F65}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F32" sqref="F32:Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="35">
+        <v>2018</v>
+      </c>
+      <c r="D1" s="35">
+        <v>2018</v>
+      </c>
+      <c r="E1" s="35">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="35">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="35">
+        <v>2019</v>
+      </c>
+      <c r="H1" s="35">
+        <v>2019</v>
+      </c>
+      <c r="I1" s="35">
+        <v>2019</v>
+      </c>
+      <c r="J1" s="35">
+        <v>2019</v>
+      </c>
+      <c r="K1" s="35">
+        <v>2019</v>
+      </c>
+      <c r="L1" s="35">
+        <v>2019</v>
+      </c>
+      <c r="M1" s="35">
+        <v>2019</v>
+      </c>
+      <c r="N1" s="35">
+        <v>2019</v>
+      </c>
+      <c r="O1" s="35">
+        <v>2019</v>
+      </c>
+      <c r="P1" s="35">
+        <v>2019</v>
+      </c>
+      <c r="Q1" s="35">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="M2" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="N2" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="O2" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="P2" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q2" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="V2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>94</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>124</v>
+      </c>
+      <c r="I3">
+        <v>87</v>
+      </c>
+      <c r="J3">
+        <v>82</v>
+      </c>
+      <c r="K3">
+        <v>96</v>
+      </c>
+      <c r="L3">
+        <v>79</v>
+      </c>
+      <c r="M3">
+        <v>80</v>
+      </c>
+      <c r="N3">
+        <v>97</v>
+      </c>
+      <c r="O3">
+        <v>102</v>
+      </c>
+      <c r="P3">
+        <v>24</v>
+      </c>
+      <c r="Q3">
+        <v>107</v>
+      </c>
+      <c r="U3" t="s">
+        <v>5</v>
+      </c>
+      <c r="V3" s="36">
+        <v>5.1350000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C4">
+        <v>121</v>
+      </c>
+      <c r="D4">
+        <v>175</v>
+      </c>
+      <c r="E4">
+        <v>150</v>
+      </c>
+      <c r="F4">
+        <v>270</v>
+      </c>
+      <c r="G4">
+        <v>294</v>
+      </c>
+      <c r="H4">
+        <v>269</v>
+      </c>
+      <c r="I4">
+        <v>232</v>
+      </c>
+      <c r="J4">
+        <v>167</v>
+      </c>
+      <c r="K4">
+        <v>140</v>
+      </c>
+      <c r="L4">
+        <v>159</v>
+      </c>
+      <c r="M4">
+        <v>245</v>
+      </c>
+      <c r="N4">
+        <v>283</v>
+      </c>
+      <c r="O4">
+        <v>291</v>
+      </c>
+      <c r="P4">
+        <v>45</v>
+      </c>
+      <c r="Q4">
+        <v>202</v>
+      </c>
+      <c r="U4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V4" s="36">
+        <v>1.0385000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>503</v>
+      </c>
+      <c r="D5">
+        <v>452</v>
+      </c>
+      <c r="E5">
+        <v>378</v>
+      </c>
+      <c r="F5">
+        <v>396</v>
+      </c>
+      <c r="G5">
+        <v>216</v>
+      </c>
+      <c r="H5">
+        <v>570</v>
+      </c>
+      <c r="I5">
+        <v>426</v>
+      </c>
+      <c r="J5">
+        <v>412</v>
+      </c>
+      <c r="K5">
+        <v>414</v>
+      </c>
+      <c r="L5">
+        <v>362</v>
+      </c>
+      <c r="M5">
+        <v>351</v>
+      </c>
+      <c r="N5">
+        <v>403</v>
+      </c>
+      <c r="O5">
+        <v>426</v>
+      </c>
+      <c r="P5">
+        <v>19</v>
+      </c>
+      <c r="Q5">
+        <v>388</v>
+      </c>
+      <c r="U5" t="s">
+        <v>21</v>
+      </c>
+      <c r="V5" s="36">
+        <v>2.7320000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>115</v>
+      </c>
+      <c r="D6">
+        <v>95</v>
+      </c>
+      <c r="E6">
+        <v>52</v>
+      </c>
+      <c r="F6">
+        <v>145</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>110</v>
+      </c>
+      <c r="I6">
+        <v>104</v>
+      </c>
+      <c r="J6">
+        <v>83</v>
+      </c>
+      <c r="K6">
+        <v>89</v>
+      </c>
+      <c r="L6">
+        <v>74</v>
+      </c>
+      <c r="M6">
+        <v>79</v>
+      </c>
+      <c r="N6">
+        <v>78</v>
+      </c>
+      <c r="O6">
+        <v>86</v>
+      </c>
+      <c r="P6">
+        <v>46</v>
+      </c>
+      <c r="Q6">
+        <v>61</v>
+      </c>
+      <c r="U6" t="s">
+        <v>25</v>
+      </c>
+      <c r="V6" s="36">
+        <v>4.8800000000000008</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>23</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="I7">
+        <v>16</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>26</v>
+      </c>
+      <c r="L7">
+        <v>129</v>
+      </c>
+      <c r="M7">
+        <v>173</v>
+      </c>
+      <c r="N7">
+        <v>191</v>
+      </c>
+      <c r="O7">
+        <v>247</v>
+      </c>
+      <c r="P7">
+        <v>79</v>
+      </c>
+      <c r="Q7">
+        <v>201</v>
+      </c>
+      <c r="U7" t="s">
+        <v>29</v>
+      </c>
+      <c r="V7" s="36">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8">
+        <v>300</v>
+      </c>
+      <c r="D8">
+        <v>275</v>
+      </c>
+      <c r="E8">
+        <v>126</v>
+      </c>
+      <c r="F8">
+        <v>184</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>173</v>
+      </c>
+      <c r="I8">
+        <v>117</v>
+      </c>
+      <c r="J8">
+        <v>117</v>
+      </c>
+      <c r="K8">
+        <v>121</v>
+      </c>
+      <c r="L8">
+        <v>59</v>
+      </c>
+      <c r="M8">
+        <v>75</v>
+      </c>
+      <c r="N8">
+        <v>73</v>
+      </c>
+      <c r="O8">
+        <v>69</v>
+      </c>
+      <c r="P8">
+        <v>96</v>
+      </c>
+      <c r="Q8">
+        <v>48</v>
+      </c>
+      <c r="U8" t="s">
+        <v>34</v>
+      </c>
+      <c r="V8" s="36">
+        <v>2.7500000000000009</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9">
+        <v>302</v>
+      </c>
+      <c r="D9">
+        <v>281</v>
+      </c>
+      <c r="E9">
+        <v>137</v>
+      </c>
+      <c r="F9">
+        <v>183</v>
+      </c>
+      <c r="G9">
+        <v>48</v>
+      </c>
+      <c r="H9">
+        <v>176</v>
+      </c>
+      <c r="I9">
+        <v>169</v>
+      </c>
+      <c r="J9">
+        <v>119</v>
+      </c>
+      <c r="K9">
+        <v>96</v>
+      </c>
+      <c r="L9">
+        <v>85</v>
+      </c>
+      <c r="M9">
+        <v>77</v>
+      </c>
+      <c r="N9">
+        <v>110</v>
+      </c>
+      <c r="O9">
+        <v>119</v>
+      </c>
+      <c r="P9">
+        <v>37</v>
+      </c>
+      <c r="Q9">
+        <v>52</v>
+      </c>
+      <c r="U9" t="s">
+        <v>36</v>
+      </c>
+      <c r="V9" s="36">
+        <v>2.0600000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10">
+        <v>206</v>
+      </c>
+      <c r="D10">
+        <v>163</v>
+      </c>
+      <c r="E10">
+        <v>133</v>
+      </c>
+      <c r="F10">
+        <v>149</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>159</v>
+      </c>
+      <c r="I10">
+        <v>134</v>
+      </c>
+      <c r="J10">
+        <v>111</v>
+      </c>
+      <c r="K10">
+        <v>97</v>
+      </c>
+      <c r="L10">
+        <v>93</v>
+      </c>
+      <c r="M10">
+        <v>95</v>
+      </c>
+      <c r="N10">
+        <v>112</v>
+      </c>
+      <c r="O10">
+        <v>85</v>
+      </c>
+      <c r="P10">
+        <v>52</v>
+      </c>
+      <c r="Q10">
+        <v>77</v>
+      </c>
+      <c r="U10" t="s">
+        <v>38</v>
+      </c>
+      <c r="V10" s="36">
+        <v>1.9720000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>14</v>
+      </c>
+      <c r="I11">
+        <v>8</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>15</v>
+      </c>
+      <c r="L11">
+        <v>57</v>
+      </c>
+      <c r="M11">
+        <v>80</v>
+      </c>
+      <c r="N11">
+        <v>50</v>
+      </c>
+      <c r="O11">
+        <v>74</v>
+      </c>
+      <c r="P11">
+        <v>6</v>
+      </c>
+      <c r="Q11">
+        <v>65</v>
+      </c>
+      <c r="U11" t="s">
+        <v>43</v>
+      </c>
+      <c r="V11" s="36">
+        <v>2.052</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12">
+        <v>81</v>
+      </c>
+      <c r="D12">
+        <v>77</v>
+      </c>
+      <c r="E12">
+        <v>87</v>
+      </c>
+      <c r="F12">
+        <v>106</v>
+      </c>
+      <c r="G12">
+        <v>48</v>
+      </c>
+      <c r="H12">
+        <v>111</v>
+      </c>
+      <c r="I12">
+        <v>100</v>
+      </c>
+      <c r="J12">
+        <v>90</v>
+      </c>
+      <c r="K12">
+        <v>78</v>
+      </c>
+      <c r="L12">
+        <v>96</v>
+      </c>
+      <c r="M12">
+        <v>103</v>
+      </c>
+      <c r="N12">
+        <v>101</v>
+      </c>
+      <c r="O12">
+        <v>100</v>
+      </c>
+      <c r="P12">
+        <v>52</v>
+      </c>
+      <c r="Q12">
+        <v>95</v>
+      </c>
+      <c r="U12" t="s">
+        <v>46</v>
+      </c>
+      <c r="V12" s="36">
+        <v>2.3945000000000007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>49</v>
       </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>141</v>
+      </c>
+      <c r="D13">
+        <v>148</v>
+      </c>
+      <c r="E13">
+        <v>137</v>
+      </c>
+      <c r="F13">
+        <v>193</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>261</v>
+      </c>
+      <c r="I13">
+        <v>215</v>
+      </c>
+      <c r="J13">
+        <v>199</v>
+      </c>
+      <c r="K13">
+        <v>133</v>
+      </c>
+      <c r="L13">
+        <v>36</v>
+      </c>
+      <c r="M13">
+        <v>47</v>
+      </c>
+      <c r="N13">
+        <v>36</v>
+      </c>
+      <c r="O13">
+        <v>31</v>
+      </c>
+      <c r="P13">
+        <v>112</v>
+      </c>
+      <c r="Q13">
+        <v>36</v>
+      </c>
+      <c r="U13" t="s">
+        <v>49</v>
+      </c>
+      <c r="V13" s="36">
+        <v>2.7444999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="34"/>
+      <c r="C17" s="35">
+        <v>2018</v>
+      </c>
+      <c r="D17" s="35">
+        <v>2018</v>
+      </c>
+      <c r="E17" s="35">
+        <v>2018</v>
+      </c>
+      <c r="F17" s="35">
+        <v>2019</v>
+      </c>
+      <c r="G17" s="35">
+        <v>2019</v>
+      </c>
+      <c r="H17" s="35">
+        <v>2019</v>
+      </c>
+      <c r="I17" s="35">
+        <v>2019</v>
+      </c>
+      <c r="J17" s="35">
+        <v>2019</v>
+      </c>
+      <c r="K17" s="35">
+        <v>2019</v>
+      </c>
+      <c r="L17" s="35">
+        <v>2019</v>
+      </c>
+      <c r="M17" s="35">
+        <v>2019</v>
+      </c>
+      <c r="N17" s="35">
+        <v>2019</v>
+      </c>
+      <c r="O17" s="35">
+        <v>2019</v>
+      </c>
+      <c r="P17" s="35">
+        <v>2019</v>
+      </c>
+      <c r="Q17" s="35">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="J18" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="K18" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="L18" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="M18" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="N18" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="O18" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="P18" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q18" s="35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="36">
+        <f>C3*$V3</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="36">
+        <f t="shared" ref="D19:Q19" si="0">D3*$V3</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="36">
+        <f t="shared" si="0"/>
+        <v>482.69000000000005</v>
+      </c>
+      <c r="G19" s="36">
+        <f t="shared" si="0"/>
+        <v>51.350000000000009</v>
+      </c>
+      <c r="H19" s="36">
+        <f t="shared" si="0"/>
+        <v>636.74000000000012</v>
+      </c>
+      <c r="I19" s="36">
+        <f t="shared" si="0"/>
+        <v>446.74500000000006</v>
+      </c>
+      <c r="J19" s="36">
+        <f t="shared" si="0"/>
+        <v>421.07000000000005</v>
+      </c>
+      <c r="K19" s="36">
+        <f t="shared" si="0"/>
+        <v>492.96000000000004</v>
+      </c>
+      <c r="L19" s="36">
+        <f t="shared" si="0"/>
+        <v>405.66500000000008</v>
+      </c>
+      <c r="M19" s="36">
+        <f t="shared" si="0"/>
+        <v>410.80000000000007</v>
+      </c>
+      <c r="N19" s="36">
+        <f t="shared" si="0"/>
+        <v>498.09500000000008</v>
+      </c>
+      <c r="O19" s="36">
+        <f t="shared" si="0"/>
+        <v>523.7700000000001</v>
+      </c>
+      <c r="P19" s="36">
+        <f t="shared" si="0"/>
+        <v>123.24000000000001</v>
+      </c>
+      <c r="Q19" s="36">
+        <f t="shared" si="0"/>
+        <v>549.44500000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="36">
+        <f t="shared" ref="C20:Q29" si="1">C4*$V4</f>
+        <v>125.65850000000002</v>
+      </c>
+      <c r="D20" s="36">
+        <f t="shared" si="1"/>
+        <v>181.73750000000004</v>
+      </c>
+      <c r="E20" s="36">
+        <f t="shared" si="1"/>
+        <v>155.77500000000003</v>
+      </c>
+      <c r="F20" s="36">
+        <f t="shared" si="1"/>
+        <v>280.39500000000004</v>
+      </c>
+      <c r="G20" s="36">
+        <f t="shared" si="1"/>
+        <v>305.31900000000007</v>
+      </c>
+      <c r="H20" s="36">
+        <f t="shared" si="1"/>
+        <v>279.35650000000004</v>
+      </c>
+      <c r="I20" s="36">
+        <f t="shared" si="1"/>
+        <v>240.93200000000004</v>
+      </c>
+      <c r="J20" s="36">
+        <f t="shared" si="1"/>
+        <v>173.42950000000005</v>
+      </c>
+      <c r="K20" s="36">
+        <f t="shared" si="1"/>
+        <v>145.39000000000001</v>
+      </c>
+      <c r="L20" s="36">
+        <f t="shared" si="1"/>
+        <v>165.12150000000003</v>
+      </c>
+      <c r="M20" s="36">
+        <f t="shared" si="1"/>
+        <v>254.43250000000006</v>
+      </c>
+      <c r="N20" s="36">
+        <f t="shared" si="1"/>
+        <v>293.89550000000008</v>
+      </c>
+      <c r="O20" s="36">
+        <f t="shared" si="1"/>
+        <v>302.20350000000008</v>
+      </c>
+      <c r="P20" s="36">
+        <f t="shared" si="1"/>
+        <v>46.732500000000009</v>
+      </c>
+      <c r="Q20" s="36">
+        <f t="shared" si="1"/>
+        <v>209.77700000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="36">
+        <f t="shared" si="1"/>
+        <v>1374.1960000000001</v>
+      </c>
+      <c r="D21" s="36">
+        <f t="shared" si="1"/>
+        <v>1234.864</v>
+      </c>
+      <c r="E21" s="36">
+        <f t="shared" si="1"/>
+        <v>1032.6960000000001</v>
+      </c>
+      <c r="F21" s="36">
+        <f t="shared" si="1"/>
+        <v>1081.8720000000001</v>
+      </c>
+      <c r="G21" s="36">
+        <f t="shared" si="1"/>
+        <v>590.11200000000008</v>
+      </c>
+      <c r="H21" s="36">
+        <f t="shared" si="1"/>
+        <v>1557.24</v>
+      </c>
+      <c r="I21" s="36">
+        <f t="shared" si="1"/>
+        <v>1163.8320000000001</v>
+      </c>
+      <c r="J21" s="36">
+        <f t="shared" si="1"/>
+        <v>1125.5840000000001</v>
+      </c>
+      <c r="K21" s="36">
+        <f t="shared" si="1"/>
+        <v>1131.048</v>
+      </c>
+      <c r="L21" s="36">
+        <f t="shared" si="1"/>
+        <v>988.98400000000004</v>
+      </c>
+      <c r="M21" s="36">
+        <f t="shared" si="1"/>
+        <v>958.93200000000002</v>
+      </c>
+      <c r="N21" s="36">
+        <f t="shared" si="1"/>
+        <v>1100.9960000000001</v>
+      </c>
+      <c r="O21" s="36">
+        <f t="shared" si="1"/>
+        <v>1163.8320000000001</v>
+      </c>
+      <c r="P21" s="36">
+        <f t="shared" si="1"/>
+        <v>51.908000000000001</v>
+      </c>
+      <c r="Q21" s="36">
+        <f t="shared" si="1"/>
+        <v>1060.0160000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="36">
+        <f t="shared" si="1"/>
+        <v>561.20000000000005</v>
+      </c>
+      <c r="D22" s="36">
+        <f t="shared" si="1"/>
+        <v>463.60000000000008</v>
+      </c>
+      <c r="E22" s="36">
+        <f t="shared" si="1"/>
+        <v>253.76000000000005</v>
+      </c>
+      <c r="F22" s="36">
+        <f t="shared" si="1"/>
+        <v>707.60000000000014</v>
+      </c>
+      <c r="G22" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="36">
+        <f t="shared" si="1"/>
+        <v>536.80000000000007</v>
+      </c>
+      <c r="I22" s="36">
+        <f t="shared" si="1"/>
+        <v>507.5200000000001</v>
+      </c>
+      <c r="J22" s="36">
+        <f t="shared" si="1"/>
+        <v>405.04000000000008</v>
+      </c>
+      <c r="K22" s="36">
+        <f t="shared" si="1"/>
+        <v>434.32000000000005</v>
+      </c>
+      <c r="L22" s="36">
+        <f t="shared" si="1"/>
+        <v>361.12000000000006</v>
+      </c>
+      <c r="M22" s="36">
+        <f t="shared" si="1"/>
+        <v>385.52000000000004</v>
+      </c>
+      <c r="N22" s="36">
+        <f t="shared" si="1"/>
+        <v>380.64000000000004</v>
+      </c>
+      <c r="O22" s="36">
+        <f t="shared" si="1"/>
+        <v>419.68000000000006</v>
+      </c>
+      <c r="P22" s="36">
+        <f t="shared" si="1"/>
+        <v>224.48000000000005</v>
+      </c>
+      <c r="Q22" s="36">
+        <f t="shared" si="1"/>
+        <v>297.68000000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="36">
+        <f t="shared" si="1"/>
+        <v>34.729999999999997</v>
+      </c>
+      <c r="H23" s="36">
+        <f t="shared" si="1"/>
+        <v>30.2</v>
+      </c>
+      <c r="I23" s="36">
+        <f t="shared" si="1"/>
+        <v>24.16</v>
+      </c>
+      <c r="J23" s="36">
+        <f t="shared" si="1"/>
+        <v>3.02</v>
+      </c>
+      <c r="K23" s="36">
+        <f t="shared" si="1"/>
+        <v>39.26</v>
+      </c>
+      <c r="L23" s="36">
+        <f t="shared" si="1"/>
+        <v>194.79</v>
+      </c>
+      <c r="M23" s="36">
+        <f t="shared" si="1"/>
+        <v>261.23</v>
+      </c>
+      <c r="N23" s="36">
+        <f t="shared" si="1"/>
+        <v>288.41000000000003</v>
+      </c>
+      <c r="O23" s="36">
+        <f t="shared" si="1"/>
+        <v>372.97</v>
+      </c>
+      <c r="P23" s="36">
+        <f t="shared" si="1"/>
+        <v>119.29</v>
+      </c>
+      <c r="Q23" s="36">
+        <f t="shared" si="1"/>
+        <v>303.51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="36">
+        <f t="shared" si="1"/>
+        <v>825.00000000000023</v>
+      </c>
+      <c r="D24" s="36">
+        <f t="shared" si="1"/>
+        <v>756.25000000000023</v>
+      </c>
+      <c r="E24" s="36">
+        <f t="shared" si="1"/>
+        <v>346.50000000000011</v>
+      </c>
+      <c r="F24" s="36">
+        <f t="shared" si="1"/>
+        <v>506.00000000000017</v>
+      </c>
+      <c r="G24" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="36">
+        <f t="shared" si="1"/>
+        <v>475.75000000000017</v>
+      </c>
+      <c r="I24" s="36">
+        <f t="shared" si="1"/>
+        <v>321.75000000000011</v>
+      </c>
+      <c r="J24" s="36">
+        <f t="shared" si="1"/>
+        <v>321.75000000000011</v>
+      </c>
+      <c r="K24" s="36">
+        <f t="shared" si="1"/>
+        <v>332.75000000000011</v>
+      </c>
+      <c r="L24" s="36">
+        <f t="shared" si="1"/>
+        <v>162.25000000000006</v>
+      </c>
+      <c r="M24" s="36">
+        <f t="shared" si="1"/>
+        <v>206.25000000000006</v>
+      </c>
+      <c r="N24" s="36">
+        <f t="shared" si="1"/>
+        <v>200.75000000000006</v>
+      </c>
+      <c r="O24" s="36">
+        <f t="shared" si="1"/>
+        <v>189.75000000000006</v>
+      </c>
+      <c r="P24" s="36">
+        <f t="shared" si="1"/>
+        <v>264.00000000000011</v>
+      </c>
+      <c r="Q24" s="36">
+        <f t="shared" si="1"/>
+        <v>132.00000000000006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="36">
+        <f t="shared" si="1"/>
+        <v>622.12000000000012</v>
+      </c>
+      <c r="D25" s="36">
+        <f t="shared" si="1"/>
+        <v>578.86000000000013</v>
+      </c>
+      <c r="E25" s="36">
+        <f t="shared" si="1"/>
+        <v>282.22000000000008</v>
+      </c>
+      <c r="F25" s="36">
+        <f t="shared" si="1"/>
+        <v>376.98000000000008</v>
+      </c>
+      <c r="G25" s="36">
+        <f t="shared" si="1"/>
+        <v>98.880000000000024</v>
+      </c>
+      <c r="H25" s="36">
+        <f t="shared" si="1"/>
+        <v>362.56000000000006</v>
+      </c>
+      <c r="I25" s="36">
+        <f t="shared" si="1"/>
+        <v>348.1400000000001</v>
+      </c>
+      <c r="J25" s="36">
+        <f t="shared" si="1"/>
+        <v>245.14000000000007</v>
+      </c>
+      <c r="K25" s="36">
+        <f t="shared" si="1"/>
+        <v>197.76000000000005</v>
+      </c>
+      <c r="L25" s="36">
+        <f t="shared" si="1"/>
+        <v>175.10000000000005</v>
+      </c>
+      <c r="M25" s="36">
+        <f t="shared" si="1"/>
+        <v>158.62000000000003</v>
+      </c>
+      <c r="N25" s="36">
+        <f t="shared" si="1"/>
+        <v>226.60000000000005</v>
+      </c>
+      <c r="O25" s="36">
+        <f t="shared" si="1"/>
+        <v>245.14000000000007</v>
+      </c>
+      <c r="P25" s="36">
+        <f t="shared" si="1"/>
+        <v>76.220000000000013</v>
+      </c>
+      <c r="Q25" s="36">
+        <f t="shared" si="1"/>
+        <v>107.12000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="36">
+        <f t="shared" si="1"/>
+        <v>406.23200000000003</v>
+      </c>
+      <c r="D26" s="36">
+        <f t="shared" si="1"/>
+        <v>321.43600000000004</v>
+      </c>
+      <c r="E26" s="36">
+        <f t="shared" si="1"/>
+        <v>262.27600000000001</v>
+      </c>
+      <c r="F26" s="36">
+        <f t="shared" si="1"/>
+        <v>293.82800000000003</v>
+      </c>
+      <c r="G26" s="36">
+        <f t="shared" si="1"/>
+        <v>7.8880000000000008</v>
+      </c>
+      <c r="H26" s="36">
+        <f t="shared" si="1"/>
+        <v>313.54800000000006</v>
+      </c>
+      <c r="I26" s="36">
+        <f t="shared" si="1"/>
+        <v>264.24800000000005</v>
+      </c>
+      <c r="J26" s="36">
+        <f t="shared" si="1"/>
+        <v>218.89200000000002</v>
+      </c>
+      <c r="K26" s="36">
+        <f t="shared" si="1"/>
+        <v>191.28400000000002</v>
+      </c>
+      <c r="L26" s="36">
+        <f t="shared" si="1"/>
+        <v>183.39600000000002</v>
+      </c>
+      <c r="M26" s="36">
+        <f t="shared" si="1"/>
+        <v>187.34000000000003</v>
+      </c>
+      <c r="N26" s="36">
+        <f t="shared" si="1"/>
+        <v>220.86400000000003</v>
+      </c>
+      <c r="O26" s="36">
+        <f t="shared" si="1"/>
+        <v>167.62</v>
+      </c>
+      <c r="P26" s="36">
+        <f t="shared" si="1"/>
+        <v>102.54400000000001</v>
+      </c>
+      <c r="Q26" s="36">
+        <f t="shared" si="1"/>
+        <v>151.84400000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="36">
+        <f t="shared" si="1"/>
+        <v>10.26</v>
+      </c>
+      <c r="H27" s="36">
+        <f t="shared" si="1"/>
+        <v>28.728000000000002</v>
+      </c>
+      <c r="I27" s="36">
+        <f t="shared" si="1"/>
+        <v>16.416</v>
+      </c>
+      <c r="J27" s="36">
+        <f t="shared" si="1"/>
+        <v>4.1040000000000001</v>
+      </c>
+      <c r="K27" s="36">
+        <f t="shared" si="1"/>
+        <v>30.78</v>
+      </c>
+      <c r="L27" s="36">
+        <f t="shared" si="1"/>
+        <v>116.964</v>
+      </c>
+      <c r="M27" s="36">
+        <f t="shared" si="1"/>
+        <v>164.16</v>
+      </c>
+      <c r="N27" s="36">
+        <f t="shared" si="1"/>
+        <v>102.60000000000001</v>
+      </c>
+      <c r="O27" s="36">
+        <f t="shared" si="1"/>
+        <v>151.84800000000001</v>
+      </c>
+      <c r="P27" s="36">
+        <f t="shared" si="1"/>
+        <v>12.312000000000001</v>
+      </c>
+      <c r="Q27" s="36">
+        <f t="shared" si="1"/>
+        <v>133.38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="36">
+        <f t="shared" si="1"/>
+        <v>193.95450000000005</v>
+      </c>
+      <c r="D28" s="36">
+        <f t="shared" si="1"/>
+        <v>184.37650000000005</v>
+      </c>
+      <c r="E28" s="36">
+        <f t="shared" si="1"/>
+        <v>208.32150000000007</v>
+      </c>
+      <c r="F28" s="36">
+        <f t="shared" si="1"/>
+        <v>253.81700000000006</v>
+      </c>
+      <c r="G28" s="36">
+        <f t="shared" si="1"/>
+        <v>114.93600000000004</v>
+      </c>
+      <c r="H28" s="36">
+        <f t="shared" si="1"/>
+        <v>265.78950000000009</v>
+      </c>
+      <c r="I28" s="36">
+        <f t="shared" si="1"/>
+        <v>239.45000000000007</v>
+      </c>
+      <c r="J28" s="36">
+        <f t="shared" si="1"/>
+        <v>215.50500000000005</v>
+      </c>
+      <c r="K28" s="36">
+        <f t="shared" si="1"/>
+        <v>186.77100000000007</v>
+      </c>
+      <c r="L28" s="36">
+        <f t="shared" si="1"/>
+        <v>229.87200000000007</v>
+      </c>
+      <c r="M28" s="36">
+        <f t="shared" si="1"/>
+        <v>246.63350000000008</v>
+      </c>
+      <c r="N28" s="36">
+        <f t="shared" si="1"/>
+        <v>241.84450000000007</v>
+      </c>
+      <c r="O28" s="36">
+        <f t="shared" si="1"/>
+        <v>239.45000000000007</v>
+      </c>
+      <c r="P28" s="36">
+        <f t="shared" si="1"/>
+        <v>124.51400000000004</v>
+      </c>
+      <c r="Q28" s="36">
+        <f t="shared" si="1"/>
+        <v>227.47750000000008</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="36">
+        <f t="shared" si="1"/>
+        <v>386.97449999999992</v>
+      </c>
+      <c r="D29" s="36">
+        <f t="shared" si="1"/>
+        <v>406.18599999999992</v>
+      </c>
+      <c r="E29" s="36">
+        <f t="shared" si="1"/>
+        <v>375.99649999999991</v>
+      </c>
+      <c r="F29" s="36">
+        <f t="shared" si="1"/>
+        <v>529.68849999999986</v>
+      </c>
+      <c r="G29" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="36">
+        <f t="shared" si="1"/>
+        <v>716.31449999999984</v>
+      </c>
+      <c r="I29" s="36">
+        <f t="shared" si="1"/>
+        <v>590.06749999999988</v>
+      </c>
+      <c r="J29" s="36">
+        <f t="shared" si="1"/>
+        <v>546.15549999999985</v>
+      </c>
+      <c r="K29" s="36">
+        <f t="shared" si="1"/>
+        <v>365.01849999999996</v>
+      </c>
+      <c r="L29" s="36">
+        <f t="shared" si="1"/>
+        <v>98.801999999999978</v>
+      </c>
+      <c r="M29" s="36">
+        <f t="shared" si="1"/>
+        <v>128.99149999999997</v>
+      </c>
+      <c r="N29" s="36">
+        <f t="shared" si="1"/>
+        <v>98.801999999999978</v>
+      </c>
+      <c r="O29" s="36">
+        <f t="shared" si="1"/>
+        <v>85.079499999999982</v>
+      </c>
+      <c r="P29" s="36">
+        <f t="shared" si="1"/>
+        <v>307.38399999999996</v>
+      </c>
+      <c r="Q29" s="36">
+        <f t="shared" si="1"/>
+        <v>98.801999999999978</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="36">
+        <f>SUM(C19:C25)</f>
+        <v>3508.1745000000001</v>
+      </c>
+      <c r="D31" s="36">
+        <f t="shared" ref="D31:Q31" si="2">SUM(D19:D25)</f>
+        <v>3215.3115000000003</v>
+      </c>
+      <c r="E31" s="36">
+        <f t="shared" si="2"/>
+        <v>2070.9510000000005</v>
+      </c>
+      <c r="F31" s="36">
+        <f t="shared" si="2"/>
+        <v>3435.5370000000003</v>
+      </c>
+      <c r="G31" s="36">
+        <f t="shared" si="2"/>
+        <v>1080.3910000000003</v>
+      </c>
+      <c r="H31" s="36">
+        <f t="shared" si="2"/>
+        <v>3878.6465000000003</v>
+      </c>
+      <c r="I31" s="36">
+        <f t="shared" si="2"/>
+        <v>3053.0790000000006</v>
+      </c>
+      <c r="J31" s="36">
+        <f t="shared" si="2"/>
+        <v>2695.0335</v>
+      </c>
+      <c r="K31" s="36">
+        <f t="shared" si="2"/>
+        <v>2773.4880000000007</v>
+      </c>
+      <c r="L31" s="36">
+        <f t="shared" si="2"/>
+        <v>2453.0305000000003</v>
+      </c>
+      <c r="M31" s="36">
+        <f t="shared" si="2"/>
+        <v>2635.7844999999998</v>
+      </c>
+      <c r="N31" s="36">
+        <f t="shared" si="2"/>
+        <v>2989.3865000000001</v>
+      </c>
+      <c r="O31" s="36">
+        <f t="shared" si="2"/>
+        <v>3217.3455000000008</v>
+      </c>
+      <c r="P31" s="36">
+        <f t="shared" si="2"/>
+        <v>905.87050000000022</v>
+      </c>
+      <c r="Q31" s="36">
+        <f t="shared" si="2"/>
+        <v>2659.5480000000007</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="36">
+        <f>SUM(C26:C29)</f>
+        <v>987.16099999999994</v>
+      </c>
+      <c r="D32" s="36">
+        <f t="shared" ref="D32:Q32" si="3">SUM(D26:D29)</f>
+        <v>911.99850000000004</v>
+      </c>
+      <c r="E32" s="36">
+        <f t="shared" si="3"/>
+        <v>846.59400000000005</v>
+      </c>
+      <c r="F32" s="36">
+        <f t="shared" si="3"/>
+        <v>1077.3335</v>
+      </c>
+      <c r="G32" s="36">
+        <f t="shared" si="3"/>
+        <v>133.08400000000003</v>
+      </c>
+      <c r="H32" s="36">
+        <f t="shared" si="3"/>
+        <v>1324.38</v>
+      </c>
+      <c r="I32" s="36">
+        <f t="shared" si="3"/>
+        <v>1110.1815000000001</v>
+      </c>
+      <c r="J32" s="36">
+        <f t="shared" si="3"/>
+        <v>984.65649999999994</v>
+      </c>
+      <c r="K32" s="36">
+        <f t="shared" si="3"/>
+        <v>773.85350000000005</v>
+      </c>
+      <c r="L32" s="36">
+        <f t="shared" si="3"/>
+        <v>629.03400000000011</v>
+      </c>
+      <c r="M32" s="36">
+        <f t="shared" si="3"/>
+        <v>727.12500000000011</v>
+      </c>
+      <c r="N32" s="36">
+        <f t="shared" si="3"/>
+        <v>664.11050000000012</v>
+      </c>
+      <c r="O32" s="36">
+        <f t="shared" si="3"/>
+        <v>643.99750000000006</v>
+      </c>
+      <c r="P32" s="36">
+        <f t="shared" si="3"/>
+        <v>546.75400000000002</v>
+      </c>
+      <c r="Q32" s="36">
+        <f t="shared" si="3"/>
+        <v>611.50350000000014</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A17:B18"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>